<commit_message>
Line 291: drop_duplicate() error - temporarily solved
</commit_message>
<xml_diff>
--- a/applied_df_test.xlsx
+++ b/applied_df_test.xlsx
@@ -14,27 +14,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+  <si>
+    <t>['Ukraine']</t>
+  </si>
+  <si>
+    <t>['Bryansk, Ukraine, Ukrainian']</t>
+  </si>
+  <si>
+    <t>['Russia']</t>
+  </si>
+  <si>
+    <t>['Bakhmut, Donetsk, Pavlohrad, Russia, Ukraine, Ukrainian']</t>
+  </si>
+  <si>
+    <t>['Pavlohrad, Ukraine']</t>
+  </si>
+  <si>
+    <t>['Russia, Ukraine']</t>
+  </si>
+  <si>
+    <t>['Kyiv, Murmansk, Pavlohrad, Russia, Ukraine, Ukrainian']</t>
+  </si>
   <si>
     <t>['']</t>
-  </si>
-  <si>
-    <t>['Cherkasy, Russia, Uman']</t>
-  </si>
-  <si>
-    <t>['Kyiv, Russia, Ukraine']</t>
-  </si>
-  <si>
-    <t>['Ukraine']</t>
-  </si>
-  <si>
-    <t>['Cape Town, South Africa']</t>
-  </si>
-  <si>
-    <t>['Russia, Ukraine']</t>
-  </si>
-  <si>
-    <t>['Western Cape']</t>
   </si>
 </sst>
 </file>
@@ -392,7 +395,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -408,156 +411,90 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1">
-        <v>82</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="1">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="1">
-        <v>63</v>
+        <v>96</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="1">
-        <v>51</v>
-      </c>
-      <c r="B10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C10" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="1">
-        <v>50</v>
-      </c>
-      <c r="B11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="1">
-        <v>17</v>
-      </c>
-      <c r="B12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="1">
-        <v>52</v>
-      </c>
-      <c r="B13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="1">
-        <v>75</v>
-      </c>
-      <c r="B14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="1">
-        <v>4</v>
-      </c>
-      <c r="B15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>